<commit_message>
Just so much Stupidity. Export in Working Condition.
</commit_message>
<xml_diff>
--- a/test/Excel_Test1.xlsx
+++ b/test/Excel_Test1.xlsx
@@ -376,23 +376,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -406,6 +418,29 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>2321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
         <v>6</v>
       </c>
     </row>

</xml_diff>